<commit_message>
fixed AP600 for Linux, finished OPR1000 model
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MCNP\dprk-elwr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7BD60EB-A31F-467F-9172-E4745220A9A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AABC29D-1680-4329-93CF-EF7D43E49D11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,11 +36,11 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="1">
+  <futureMetadata name="XLRICHVALUE" count="2">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -48,17 +48,27 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="1">
+  <valueMetadata count="2">
     <bk>
       <rc t="1" v="0"/>
+    </bk>
+    <bk>
+      <rc t="1" v="1"/>
     </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
   <si>
     <t>Input File</t>
   </si>
@@ -142,6 +152,12 @@
   </si>
   <si>
     <t>Fuel Rod</t>
+  </si>
+  <si>
+    <t>OPR1000</t>
+  </si>
+  <si>
+    <t>elwr-caseOPR1000-fuelA-blanket3.inp</t>
   </si>
 </sst>
 </file>
@@ -237,7 +253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -248,18 +264,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -320,9 +334,13 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
   <rv s="0">
     <v>0</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>1</v>
     <v>5</v>
   </rv>
 </rvData>
@@ -340,6 +358,7 @@
 <file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
 <richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <rel r:id="rId1"/>
+  <rel r:id="rId2"/>
 </richValueRels>
 </file>
 
@@ -606,17 +625,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V11"/>
+  <dimension ref="A1:V14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W23" sqref="W23"/>
+      <selection activeCell="T25" sqref="T25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34.33203125" customWidth="1"/>
     <col min="2" max="2" width="8.88671875" style="7"/>
-    <col min="3" max="3" width="10" style="10" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
     <col min="4" max="4" width="8.88671875" style="7"/>
     <col min="7" max="7" width="8.88671875" style="7"/>
     <col min="8" max="8" width="6.21875" customWidth="1"/>
@@ -633,92 +652,40 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
+      <c r="B1"/>
+      <c r="D1"/>
+      <c r="G1"/>
+      <c r="M1"/>
+      <c r="S1"/>
+      <c r="T1"/>
+      <c r="V1"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="B2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="10"/>
+      <c r="B2"/>
+      <c r="D2"/>
+      <c r="G2"/>
+      <c r="M2"/>
+      <c r="S2"/>
+      <c r="T2"/>
+      <c r="V2"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="B3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
-      <c r="V3" s="10"/>
+      <c r="B3"/>
+      <c r="D3"/>
+      <c r="G3"/>
+      <c r="M3"/>
+      <c r="S3"/>
+      <c r="T3"/>
+      <c r="V3"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="B4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
-      <c r="V4" s="10"/>
+      <c r="B4"/>
+      <c r="D4"/>
+      <c r="G4"/>
+      <c r="M4"/>
+      <c r="S4"/>
+      <c r="T4"/>
+      <c r="V4"/>
     </row>
     <row r="5" spans="1:22" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:22" x14ac:dyDescent="0.3">
@@ -740,7 +707,7 @@
         <v>10</v>
       </c>
       <c r="R6" s="3"/>
-      <c r="S6" s="12" t="s">
+      <c r="S6" s="11" t="s">
         <v>15</v>
       </c>
       <c r="T6" s="8" t="s">
@@ -755,7 +722,7 @@
       <c r="B7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="9" t="s">
@@ -803,7 +770,7 @@
       <c r="R7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="S7" s="13" t="s">
+      <c r="S7" s="12" t="s">
         <v>4</v>
       </c>
       <c r="T7" s="9" t="s">
@@ -820,10 +787,10 @@
       <c r="A8" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="15">
         <v>1.23</v>
       </c>
       <c r="D8" s="7">
@@ -848,11 +815,11 @@
       <c r="J8">
         <v>108</v>
       </c>
-      <c r="K8" s="11">
+      <c r="K8" s="10">
         <f>F8*J8*I8*((H8*235+(1-H8)*238)/((H8*235+(1-H8)*238)+2*16))</f>
         <v>203289.89088492587</v>
       </c>
-      <c r="L8" s="11">
+      <c r="L8" s="10">
         <f>F8*J8</f>
         <v>24278.644651890612</v>
       </c>
@@ -860,7 +827,7 @@
         <v>7</v>
       </c>
       <c r="N8">
-        <v>7.0229999999999997E-3</v>
+        <v>7.2040000000000003E-3</v>
       </c>
       <c r="O8">
         <v>9.5</v>
@@ -868,22 +835,22 @@
       <c r="P8">
         <v>156</v>
       </c>
-      <c r="Q8" s="11">
+      <c r="Q8" s="10">
         <f>F8*P8*O8*((N8*235+(1-N8)*238)/((N8*235+(1-N8)*238)+2*16))</f>
-        <v>293668.60676235752</v>
-      </c>
-      <c r="R8" s="11">
+        <v>293668.52734053996</v>
+      </c>
+      <c r="R8" s="10">
         <f>F8*P8</f>
         <v>35069.153386064223</v>
       </c>
-      <c r="S8" s="14">
+      <c r="S8" s="13">
         <f>L8+R8</f>
         <v>59347.798037954839</v>
       </c>
       <c r="T8" s="7">
         <v>28.361339999999998</v>
       </c>
-      <c r="V8" s="19" t="e" vm="1">
+      <c r="V8" s="16" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
     </row>
@@ -891,10 +858,10 @@
       <c r="A9" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="15">
         <v>1.23</v>
       </c>
       <c r="D9" s="7">
@@ -916,54 +883,45 @@
       <c r="I9">
         <v>9.5</v>
       </c>
-      <c r="J9">
-        <v>108</v>
-      </c>
-      <c r="K9" s="11">
+      <c r="K9" s="10">
         <f>F9*J9*I9*((H9*235+(1-H9)*238)/((H9*235+(1-H9)*238)+2*16))</f>
-        <v>203289.89088492587</v>
-      </c>
-      <c r="L9" s="11">
+        <v>0</v>
+      </c>
+      <c r="L9" s="10">
         <f>F9*J9</f>
-        <v>24278.644651890612</v>
+        <v>0</v>
       </c>
       <c r="M9" s="7" t="s">
         <v>22</v>
       </c>
       <c r="N9">
-        <v>7.0229999999999997E-3</v>
+        <v>7.2040000000000003E-3</v>
       </c>
       <c r="O9">
         <v>18.5</v>
       </c>
-      <c r="P9">
-        <v>156</v>
-      </c>
-      <c r="Q9" s="11">
+      <c r="Q9" s="10">
         <f>F9*P9*O9*((N9*235+(1-N9)*238)/((N9*235+(1-N9)*238)+2*16))</f>
-        <v>571880.97106353834</v>
-      </c>
-      <c r="R9" s="11">
+        <v>0</v>
+      </c>
+      <c r="R9" s="10">
         <f>F9*P9</f>
-        <v>35069.153386064223</v>
-      </c>
-      <c r="S9" s="14">
+        <v>0</v>
+      </c>
+      <c r="S9" s="13">
         <f>L9+R9</f>
-        <v>59347.798037954839</v>
-      </c>
-      <c r="T9" s="7">
-        <v>28.361339999999998</v>
-      </c>
-      <c r="V9" s="18"/>
+        <v>0</v>
+      </c>
+      <c r="V9" s="17"/>
     </row>
     <row r="10" spans="1:22" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="15">
         <v>1.23</v>
       </c>
       <c r="D10" s="7">
@@ -985,45 +943,36 @@
       <c r="I10">
         <v>9.5</v>
       </c>
-      <c r="J10">
-        <v>108</v>
-      </c>
-      <c r="K10" s="11">
+      <c r="K10" s="10">
         <f>F10*J10*I10*((H10*235+(1-H10)*238)/((H10*235+(1-H10)*238)+2*16))</f>
-        <v>203289.89088492587</v>
-      </c>
-      <c r="L10" s="11">
+        <v>0</v>
+      </c>
+      <c r="L10" s="10">
         <f>F10*J10</f>
-        <v>24278.644651890612</v>
+        <v>0</v>
       </c>
       <c r="M10" s="7" t="s">
         <v>7</v>
       </c>
       <c r="N10">
-        <v>7.0229999999999997E-3</v>
+        <v>7.2040000000000003E-3</v>
       </c>
       <c r="O10">
         <v>9.5</v>
       </c>
-      <c r="P10">
-        <v>156</v>
-      </c>
-      <c r="Q10" s="11">
+      <c r="Q10" s="10">
         <f>F10*P10*O10*((N10*235+(1-N10)*238)/((N10*235+(1-N10)*238)+2*16))</f>
-        <v>293668.60676235752</v>
-      </c>
-      <c r="R10" s="11">
+        <v>0</v>
+      </c>
+      <c r="R10" s="10">
         <f>F10*P10</f>
-        <v>35069.153386064223</v>
-      </c>
-      <c r="S10" s="14">
+        <v>0</v>
+      </c>
+      <c r="S10" s="13">
         <f>L10+R10</f>
-        <v>59347.798037954839</v>
-      </c>
-      <c r="T10" s="7">
-        <v>28.361339999999998</v>
-      </c>
-      <c r="V10" s="19" t="e" vm="1">
+        <v>0</v>
+      </c>
+      <c r="V10" s="16" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
     </row>
@@ -1031,10 +980,10 @@
       <c r="A11" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C11" s="15">
         <v>1.23</v>
       </c>
       <c r="D11" s="7">
@@ -1056,50 +1005,116 @@
       <c r="I11">
         <v>9.5</v>
       </c>
-      <c r="J11">
-        <v>108</v>
-      </c>
-      <c r="K11" s="11">
+      <c r="K11" s="10">
         <f>F11*J11*I11*((H11*235+(1-H11)*238)/((H11*235+(1-H11)*238)+2*16))</f>
-        <v>203289.89088492587</v>
-      </c>
-      <c r="L11" s="11">
+        <v>0</v>
+      </c>
+      <c r="L11" s="10">
         <f>F11*J11</f>
-        <v>24278.644651890612</v>
+        <v>0</v>
       </c>
       <c r="M11" s="7" t="s">
         <v>22</v>
       </c>
       <c r="N11">
-        <v>7.0229999999999997E-3</v>
+        <v>7.2040000000000003E-3</v>
       </c>
       <c r="O11">
         <v>18.5</v>
       </c>
-      <c r="P11">
+      <c r="Q11" s="10">
+        <f>F11*P11*O11*((N11*235+(1-N11)*238)/((N11*235+(1-N11)*238)+2*16))</f>
+        <v>0</v>
+      </c>
+      <c r="R11" s="10">
+        <f>F11*P11</f>
+        <v>0</v>
+      </c>
+      <c r="S11" s="13">
+        <f>L11+R11</f>
+        <v>0</v>
+      </c>
+      <c r="V11" s="17"/>
+    </row>
+    <row r="13" spans="1:22" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="15">
+        <v>1.1863300000000001</v>
+      </c>
+      <c r="D13" s="7">
+        <v>0.40949999999999998</v>
+      </c>
+      <c r="E13">
+        <v>426.72</v>
+      </c>
+      <c r="F13" s="3">
+        <f>PI()*D13^2*E13</f>
+        <v>224.80226529528346</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I13">
+        <v>9.5</v>
+      </c>
+      <c r="J13">
+        <v>80</v>
+      </c>
+      <c r="K13" s="10">
+        <f>F13*J13*I13*((H13*235+(1-H13)*238)/((H13*235+(1-H13)*238)+2*16))</f>
+        <v>150585.10435920436</v>
+      </c>
+      <c r="L13" s="10">
+        <f>F13*J13</f>
+        <v>17984.181223622676</v>
+      </c>
+      <c r="M13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="N13">
+        <v>7.2040000000000003E-3</v>
+      </c>
+      <c r="O13">
+        <v>9.5</v>
+      </c>
+      <c r="P13">
         <v>156</v>
       </c>
-      <c r="Q11" s="11">
-        <f>F11*P11*O11*((N11*235+(1-N11)*238)/((N11*235+(1-N11)*238)+2*16))</f>
-        <v>571880.97106353834</v>
-      </c>
-      <c r="R11" s="11">
-        <f>F11*P11</f>
+      <c r="Q13" s="10">
+        <f>F13*P13*O13*((N13*235+(1-N13)*238)/((N13*235+(1-N13)*238)+2*16))</f>
+        <v>293668.52734053996</v>
+      </c>
+      <c r="R13" s="10">
+        <f>F13*P13</f>
         <v>35069.153386064223</v>
       </c>
-      <c r="S11" s="14">
-        <f>L11+R11</f>
-        <v>59347.798037954839</v>
-      </c>
-      <c r="T11" s="7">
+      <c r="S13" s="13">
+        <f>L13+R13</f>
+        <v>53053.334609686899</v>
+      </c>
+      <c r="T13" s="7">
         <v>28.361339999999998</v>
       </c>
-      <c r="V11" s="18"/>
+      <c r="V13" s="17" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V14" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="V8:V9"/>
     <mergeCell ref="V10:V11"/>
+    <mergeCell ref="V13:V14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
cores A and B
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MCNP\dprk-elwr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEEB7573-2AD4-461E-AD89-65A33B3A73A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99DF00EA-2FAF-4C51-B411-626DDD904B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="MCODE" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="MCODE (2)" sheetId="3" r:id="rId1"/>
+    <sheet name="MCODE" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="4">
+  <futureMetadata name="XLRICHVALUE" count="6">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -70,8 +71,22 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="4"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="5"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="4">
+  <valueMetadata count="6">
     <bk>
       <rc t="1" v="0"/>
     </bk>
@@ -84,12 +99,18 @@
     <bk>
       <rc t="1" v="3"/>
     </bk>
+    <bk>
+      <rc t="1" v="4"/>
+    </bk>
+    <bk>
+      <rc t="1" v="5"/>
+    </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="83">
   <si>
     <t>Input File</t>
   </si>
@@ -290,12 +311,64 @@
   </si>
   <si>
     <t>Rod 2</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>elwr-coreA.inp</t>
+  </si>
+  <si>
+    <t>elwr-coreB.inp</t>
+  </si>
+  <si>
+    <t>elwr-coreC.inp</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>BOL k-eff</t>
+  </si>
+  <si>
+    <t>Total Fuel</t>
+  </si>
+  <si>
+    <t>Weight [kg]</t>
+  </si>
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>of FAs</t>
+  </si>
+  <si>
+    <t>FA Picture</t>
+  </si>
+  <si>
+    <t>Subtotal PER FA</t>
+  </si>
+  <si>
+    <t>Subtotal IN CORE</t>
+  </si>
+  <si>
+    <t>Pwr density</t>
+  </si>
+  <si>
+    <t>167 days EFPO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="168" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -425,7 +498,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -445,18 +518,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -469,13 +545,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="11" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1448,7 +1527,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="4">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="6">
   <rv s="0">
     <v>0</v>
     <v>5</v>
@@ -1463,6 +1542,14 @@
   </rv>
   <rv s="0">
     <v>3</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>4</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>5</v>
     <v>5</v>
   </rv>
 </rvData>
@@ -1483,6 +1570,8 @@
   <rel r:id="rId2"/>
   <rel r:id="rId3"/>
   <rel r:id="rId4"/>
+  <rel r:id="rId5"/>
+  <rel r:id="rId6"/>
 </richValueRels>
 </file>
 
@@ -1748,10 +1837,630 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAC066E8-F6D1-4540-A521-7E3172A66DC3}">
+  <dimension ref="A1:AB28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="34.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="7"/>
+    <col min="7" max="7" width="8.88671875" style="7"/>
+    <col min="8" max="8" width="6.21875" customWidth="1"/>
+    <col min="9" max="9" width="7.44140625" customWidth="1"/>
+    <col min="11" max="11" width="12.21875" customWidth="1"/>
+    <col min="12" max="12" width="7.44140625" customWidth="1"/>
+    <col min="13" max="13" width="12.21875" customWidth="1"/>
+    <col min="14" max="14" width="7.44140625" customWidth="1"/>
+    <col min="15" max="15" width="8.88671875" style="7"/>
+    <col min="16" max="16" width="6.33203125" customWidth="1"/>
+    <col min="17" max="17" width="7.21875" customWidth="1"/>
+    <col min="19" max="19" width="9.44140625" customWidth="1"/>
+    <col min="20" max="20" width="7.77734375" customWidth="1"/>
+    <col min="21" max="21" width="12.88671875" customWidth="1"/>
+    <col min="22" max="22" width="10.33203125" customWidth="1"/>
+    <col min="23" max="23" width="6.88671875" style="7" customWidth="1"/>
+    <col min="24" max="24" width="8.6640625" style="7" customWidth="1"/>
+    <col min="25" max="25" width="11.77734375" style="7" customWidth="1"/>
+    <col min="26" max="26" width="11.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.44140625" customWidth="1"/>
+    <col min="28" max="28" width="22.21875" style="7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1"/>
+      <c r="D1"/>
+      <c r="G1"/>
+      <c r="O1"/>
+      <c r="X1"/>
+      <c r="Y1"/>
+      <c r="Z1"/>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B2"/>
+      <c r="C2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2"/>
+      <c r="E2">
+        <f>100*167/4000</f>
+        <v>4.1749999999999998</v>
+      </c>
+      <c r="G2"/>
+      <c r="O2"/>
+      <c r="X2"/>
+      <c r="Y2"/>
+      <c r="Z2"/>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B3"/>
+      <c r="D3"/>
+      <c r="G3"/>
+      <c r="O3"/>
+      <c r="X3"/>
+      <c r="Y3"/>
+      <c r="Z3"/>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B4"/>
+      <c r="D4"/>
+      <c r="G4"/>
+      <c r="O4"/>
+      <c r="X4"/>
+      <c r="Y4"/>
+      <c r="Z4"/>
+    </row>
+    <row r="5" spans="1:28" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="W5" s="32"/>
+      <c r="AB5" s="32"/>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="D6" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N6" s="3"/>
+      <c r="O6" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="V6" s="3"/>
+      <c r="W6" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="X6" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y6" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z6" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="AA6" s="1"/>
+    </row>
+    <row r="7" spans="1:28" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="O7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="S7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="T7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="U7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="V7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="W7" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="X7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y7" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z7" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA7" s="4"/>
+      <c r="AB7" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" ht="120" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="15">
+        <v>1.22766</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0.40949999999999998</v>
+      </c>
+      <c r="E8">
+        <v>144.16</v>
+      </c>
+      <c r="F8" s="3">
+        <f>PI()*D8^2*E8</f>
+        <v>75.945572190120131</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="I8">
+        <v>9.5</v>
+      </c>
+      <c r="J8">
+        <v>264</v>
+      </c>
+      <c r="K8" s="10">
+        <f>F8*J8*I8*((H8*235+(1-H8)*238)/((H8*235+(1-H8)*238)+2*16))</f>
+        <v>167888.31329069051</v>
+      </c>
+      <c r="L8" s="10">
+        <f>F8*J8</f>
+        <v>20049.631058191713</v>
+      </c>
+      <c r="M8" s="10">
+        <f>K8*W8</f>
+        <v>3525654.5791045008</v>
+      </c>
+      <c r="N8" s="10">
+        <f>L8*W8</f>
+        <v>421042.252222026</v>
+      </c>
+      <c r="O8" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>9.5</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8" s="10">
+        <f>F8*R8*Q8*((P8*235+(1-P8)*238)/((P8*235+(1-P8)*238)+2*16))</f>
+        <v>0</v>
+      </c>
+      <c r="T8" s="10">
+        <f>F8*R8</f>
+        <v>0</v>
+      </c>
+      <c r="U8" s="10">
+        <f>S8*W8</f>
+        <v>0</v>
+      </c>
+      <c r="V8" s="10">
+        <f>T8*W8</f>
+        <v>0</v>
+      </c>
+      <c r="W8" s="37">
+        <v>21</v>
+      </c>
+      <c r="X8" s="13">
+        <f>W8*(L8+T8)</f>
+        <v>421042.252222026</v>
+      </c>
+      <c r="Y8" s="13">
+        <f>(I8*L8+Q8*T8)*W8/1000</f>
+        <v>3999.9013961092464</v>
+      </c>
+      <c r="Z8" s="40">
+        <f>100000000/(W8*(K8+S8))</f>
+        <v>28.363527327001933</v>
+      </c>
+      <c r="AB8" s="7" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" ht="120" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="15">
+        <v>1.2268699999999999</v>
+      </c>
+      <c r="D9" s="7">
+        <v>0.40949999999999998</v>
+      </c>
+      <c r="E9">
+        <v>144.16</v>
+      </c>
+      <c r="F9" s="3">
+        <f>PI()*D9^2*E9</f>
+        <v>75.945572190120131</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="41">
+        <v>0.04</v>
+      </c>
+      <c r="I9">
+        <v>9.5</v>
+      </c>
+      <c r="J9">
+        <v>196</v>
+      </c>
+      <c r="K9" s="10">
+        <f>F9*J9*I9*((H9*235+(1-H9)*238)/((H9*235+(1-H9)*238)+2*16))</f>
+        <v>124643.42193135733</v>
+      </c>
+      <c r="L9" s="10">
+        <f>F9*J9</f>
+        <v>14885.332149263546</v>
+      </c>
+      <c r="M9" s="10">
+        <f>K9*W9</f>
+        <v>2617511.8605585038</v>
+      </c>
+      <c r="N9" s="10">
+        <f>L9*W9</f>
+        <v>312591.97513453447</v>
+      </c>
+      <c r="O9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="P9">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="Q9">
+        <v>9.5</v>
+      </c>
+      <c r="R9">
+        <v>68</v>
+      </c>
+      <c r="S9" s="10">
+        <f>F9*R9*Q9*((P9*235+(1-P9)*238)/((P9*235+(1-P9)*238)+2*16))</f>
+        <v>43244.799905423883</v>
+      </c>
+      <c r="T9" s="10">
+        <f>F9*R9</f>
+        <v>5164.2989089281691</v>
+      </c>
+      <c r="U9" s="10">
+        <f>S9*W9</f>
+        <v>908140.79801390157</v>
+      </c>
+      <c r="V9" s="10">
+        <f>T9*W9</f>
+        <v>108450.27708749156</v>
+      </c>
+      <c r="W9" s="37">
+        <v>21</v>
+      </c>
+      <c r="X9" s="13">
+        <f>W9*(L9+T9)</f>
+        <v>421042.252222026</v>
+      </c>
+      <c r="Y9" s="13">
+        <f>(I9*L9+Q9*T9)*W9/1000</f>
+        <v>3999.9013961092469</v>
+      </c>
+      <c r="Z9" s="40">
+        <f>100000000/(W9*(K9+S9))</f>
+        <v>28.363542777492903</v>
+      </c>
+      <c r="AB9" s="7" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" ht="120" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="15"/>
+      <c r="F10" s="3"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="10"/>
+      <c r="W10" s="37"/>
+      <c r="X10" s="13"/>
+      <c r="Y10" s="13"/>
+      <c r="Z10" s="33"/>
+    </row>
+    <row r="11" spans="1:28" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="34"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="36"/>
+      <c r="N11" s="36"/>
+      <c r="O11" s="35"/>
+      <c r="P11" s="34"/>
+      <c r="Q11" s="34"/>
+      <c r="R11" s="34"/>
+      <c r="S11" s="36"/>
+      <c r="T11" s="36"/>
+      <c r="U11" s="36"/>
+      <c r="V11" s="36"/>
+      <c r="W11" s="37"/>
+      <c r="X11" s="37"/>
+      <c r="Y11" s="37"/>
+    </row>
+    <row r="12" spans="1:28" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="36"/>
+      <c r="M12" s="36"/>
+      <c r="N12" s="36"/>
+      <c r="O12" s="35"/>
+      <c r="P12" s="34"/>
+      <c r="Q12" s="34"/>
+      <c r="R12" s="34"/>
+      <c r="S12" s="36"/>
+      <c r="T12" s="36"/>
+      <c r="U12" s="36"/>
+      <c r="V12" s="36"/>
+      <c r="W12" s="37"/>
+      <c r="X12" s="37"/>
+      <c r="Y12" s="37"/>
+    </row>
+    <row r="13" spans="1:28" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="34"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="36"/>
+      <c r="N13" s="36"/>
+      <c r="O13" s="35"/>
+      <c r="P13" s="34"/>
+      <c r="Q13" s="34"/>
+      <c r="R13" s="34"/>
+      <c r="S13" s="36"/>
+      <c r="T13" s="36"/>
+      <c r="U13" s="36"/>
+      <c r="V13" s="36"/>
+      <c r="W13" s="37"/>
+      <c r="X13" s="37"/>
+      <c r="Y13" s="37"/>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="C14" s="34"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="35"/>
+      <c r="P14" s="34"/>
+      <c r="Q14" s="34"/>
+      <c r="R14" s="34"/>
+      <c r="S14" s="34"/>
+      <c r="T14" s="34"/>
+      <c r="U14" s="34"/>
+      <c r="V14" s="34"/>
+      <c r="W14" s="35"/>
+      <c r="X14" s="35"/>
+      <c r="Y14" s="35"/>
+    </row>
+    <row r="15" spans="1:28" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="36"/>
+      <c r="L15" s="36"/>
+      <c r="M15" s="36"/>
+      <c r="N15" s="36"/>
+      <c r="O15" s="35"/>
+      <c r="P15" s="34"/>
+      <c r="Q15" s="34"/>
+      <c r="R15" s="34"/>
+      <c r="S15" s="36"/>
+      <c r="T15" s="36"/>
+      <c r="U15" s="36"/>
+      <c r="V15" s="36"/>
+      <c r="W15" s="37"/>
+      <c r="X15" s="37"/>
+      <c r="Y15" s="37"/>
+    </row>
+    <row r="16" spans="1:28" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="34"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="34"/>
+      <c r="O16" s="35"/>
+      <c r="P16" s="34"/>
+      <c r="Q16" s="34"/>
+      <c r="R16" s="34"/>
+      <c r="S16" s="34"/>
+      <c r="T16" s="34"/>
+      <c r="U16" s="34"/>
+      <c r="V16" s="34"/>
+      <c r="W16" s="35"/>
+      <c r="X16" s="35"/>
+      <c r="Y16" s="35"/>
+    </row>
+    <row r="17" spans="1:25" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="36"/>
+      <c r="L17" s="36"/>
+      <c r="M17" s="36"/>
+      <c r="N17" s="36"/>
+      <c r="O17" s="35"/>
+      <c r="P17" s="34"/>
+      <c r="Q17" s="34"/>
+      <c r="R17" s="34"/>
+      <c r="S17" s="36"/>
+      <c r="T17" s="36"/>
+      <c r="U17" s="36"/>
+      <c r="V17" s="36"/>
+      <c r="W17" s="37"/>
+      <c r="X17" s="37"/>
+      <c r="Y17" s="37"/>
+    </row>
+    <row r="18" spans="1:25" ht="52.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:25" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:25" ht="53.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B27" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B28" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
@@ -1976,7 +2685,7 @@
         <f>100000000/(238/(238+32)*4000000)</f>
         <v>28.361344537815125</v>
       </c>
-      <c r="V8" s="17" t="e" vm="1">
+      <c r="V8" s="26" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
     </row>
@@ -1987,7 +2696,6 @@
       <c r="B9" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="34"/>
       <c r="D9" s="7">
         <v>0.40949999999999998</v>
       </c>
@@ -2039,7 +2747,7 @@
         <f>L9+R9</f>
         <v>24278.644651890612</v>
       </c>
-      <c r="V9" s="18"/>
+      <c r="V9" s="27"/>
     </row>
     <row r="10" spans="1:22" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
@@ -2109,7 +2817,7 @@
         <f>100000000/(238/(238+32)*4000000)</f>
         <v>28.361344537815125</v>
       </c>
-      <c r="V10" s="17" t="e" vm="2">
+      <c r="V10" s="26" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
     </row>
@@ -2120,7 +2828,6 @@
       <c r="B11" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="34"/>
       <c r="D11" s="7">
         <v>0.40949999999999998</v>
       </c>
@@ -2172,7 +2879,7 @@
         <f>L11+R11</f>
         <v>32371.526202520818</v>
       </c>
-      <c r="V11" s="18"/>
+      <c r="V11" s="27"/>
     </row>
     <row r="12" spans="1:22" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -2181,7 +2888,6 @@
       <c r="B12" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="34"/>
       <c r="F12" s="3"/>
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
@@ -2194,7 +2900,6 @@
       <c r="A13" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="34"/>
       <c r="F13" s="3"/>
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
@@ -2271,7 +2976,7 @@
         <f>100000000/(238/(238+32)*4000000)</f>
         <v>28.361344537815125</v>
       </c>
-      <c r="V15" s="18" t="e" vm="3">
+      <c r="V15" s="27" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
     </row>
@@ -2282,7 +2987,7 @@
       <c r="B16" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="V16" s="18"/>
+      <c r="V16" s="27"/>
     </row>
     <row r="17" spans="1:22" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
@@ -2352,7 +3057,7 @@
         <f>100000000/(238/(238+32)*4000000)</f>
         <v>28.361344537815125</v>
       </c>
-      <c r="V17" s="18" t="e" vm="4">
+      <c r="V17" s="27" t="e" vm="6">
         <v>#VALUE!</v>
       </c>
     </row>
@@ -2381,7 +3086,7 @@
       <c r="O18">
         <v>18.5</v>
       </c>
-      <c r="V18" s="18"/>
+      <c r="V18" s="27"/>
     </row>
     <row r="19" spans="1:22" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
@@ -2408,7 +3113,7 @@
       <c r="O19">
         <v>9.5</v>
       </c>
-      <c r="V19" s="18"/>
+      <c r="V19" s="27"/>
     </row>
     <row r="20" spans="1:22" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
@@ -2435,7 +3140,7 @@
       <c r="O20">
         <v>18.5</v>
       </c>
-      <c r="V20" s="18"/>
+      <c r="V20" s="27"/>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B27" s="7" t="s">
@@ -2460,7 +3165,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E48A428C-A2D0-4C30-9161-4343E51EC6DC}">
   <dimension ref="A1:AY22"/>
   <sheetViews>
@@ -2493,16 +3198,16 @@
     <col min="29" max="29" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="20" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="T1" s="22"/>
-      <c r="W1" s="22"/>
-      <c r="Z1" s="22"/>
-      <c r="AC1" s="22"/>
+    <row r="1" spans="1:33" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="W1" s="20"/>
+      <c r="Z1" s="20"/>
+      <c r="AC1" s="20"/>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -2628,10 +3333,10 @@
       <c r="AC3" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="AD3" s="29" t="s">
+      <c r="AD3" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AE3" s="29" t="s">
+      <c r="AE3" s="1" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2657,14 +3362,14 @@
       <c r="G4">
         <v>0.234015</v>
       </c>
-      <c r="H4" s="32">
+      <c r="H4" s="23">
         <f>G4/0.0075</f>
         <v>31.202000000000002</v>
       </c>
-      <c r="I4" s="23">
+      <c r="I4" s="21">
         <v>0.855182</v>
       </c>
-      <c r="J4" s="19">
+      <c r="J4" s="17">
         <v>0.144818</v>
       </c>
       <c r="Q4" s="7">
@@ -2679,28 +3384,28 @@
       <c r="T4" s="7">
         <v>0</v>
       </c>
-      <c r="U4" s="31">
+      <c r="U4">
         <v>0</v>
       </c>
-      <c r="V4" s="31">
+      <c r="V4">
         <v>0</v>
       </c>
       <c r="W4" s="7">
         <v>0</v>
       </c>
-      <c r="X4" s="31">
+      <c r="X4">
         <v>0</v>
       </c>
-      <c r="Y4" s="31">
+      <c r="Y4">
         <v>0</v>
       </c>
       <c r="Z4" s="7">
         <v>0</v>
       </c>
-      <c r="AA4" s="31">
+      <c r="AA4">
         <v>0</v>
       </c>
-      <c r="AB4" s="31">
+      <c r="AB4">
         <v>0</v>
       </c>
     </row>
@@ -2726,87 +3431,87 @@
       <c r="G5">
         <v>0.218835</v>
       </c>
-      <c r="H5" s="32">
+      <c r="H5" s="23">
         <f t="shared" ref="H5:H11" si="0">G5/0.0075</f>
         <v>29.178000000000001</v>
       </c>
-      <c r="I5" s="23">
+      <c r="I5" s="21">
         <v>0.85313700000000003</v>
       </c>
-      <c r="J5" s="19">
+      <c r="J5" s="17">
         <v>0.14686299999999999</v>
       </c>
-      <c r="K5" s="23">
+      <c r="K5" s="21">
         <v>18690</v>
       </c>
-      <c r="L5" s="19">
+      <c r="L5" s="17">
         <v>1599</v>
       </c>
-      <c r="M5" s="19">
+      <c r="M5" s="17">
         <f>K5+L5</f>
         <v>20289</v>
       </c>
-      <c r="N5" s="23">
+      <c r="N5" s="21">
         <v>252200</v>
       </c>
-      <c r="O5" s="19">
+      <c r="O5" s="17">
         <v>224200</v>
       </c>
-      <c r="P5" s="19">
+      <c r="P5" s="17">
         <f>N5+O5</f>
         <v>476400</v>
       </c>
-      <c r="Q5" s="23">
+      <c r="Q5" s="21">
         <v>4.97</v>
       </c>
-      <c r="R5" s="19">
+      <c r="R5" s="17">
         <v>4.4950000000000001</v>
       </c>
-      <c r="S5" s="19">
+      <c r="S5" s="17">
         <f>Q5+R5</f>
         <v>9.4649999999999999</v>
       </c>
-      <c r="T5" s="23">
+      <c r="T5" s="21">
         <v>1.443E-2</v>
       </c>
-      <c r="U5" s="19">
+      <c r="U5" s="17">
         <v>1.6140000000000002E-2</v>
       </c>
-      <c r="V5" s="19">
+      <c r="V5" s="17">
         <f>T5+U5</f>
         <v>3.057E-2</v>
       </c>
-      <c r="W5" s="23">
+      <c r="W5" s="21">
         <v>6.0279999999999999E-5</v>
       </c>
-      <c r="X5" s="19">
+      <c r="X5" s="17">
         <v>6.7230000000000005E-5</v>
       </c>
-      <c r="Y5" s="19">
+      <c r="Y5" s="17">
         <f>W5+X5</f>
         <v>1.2751E-4</v>
       </c>
-      <c r="Z5" s="23">
+      <c r="Z5" s="21">
         <f>Q5+T5+W5</f>
         <v>4.9844902799999993</v>
       </c>
-      <c r="AA5" s="19">
+      <c r="AA5" s="17">
         <f>R5+U5+X5</f>
         <v>4.5112072300000001</v>
       </c>
-      <c r="AB5" s="19">
+      <c r="AB5" s="17">
         <f>Z5+AA5</f>
         <v>9.4956975099999994</v>
       </c>
-      <c r="AC5" s="23">
+      <c r="AC5" s="21">
         <f>Q5/Z5</f>
         <v>0.99709292642055281</v>
       </c>
-      <c r="AD5" s="30">
+      <c r="AD5" s="17">
         <f>R5/AA5</f>
         <v>0.99640734083501636</v>
       </c>
-      <c r="AE5" s="30">
+      <c r="AE5" s="17">
         <f>S5/AB5</f>
         <v>0.99676721905182097</v>
       </c>
@@ -2815,10 +3520,10 @@
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A6" s="25" t="e" vm="2">
+      <c r="A6" s="28" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
-      <c r="B6" s="26"/>
+      <c r="B6" s="29"/>
       <c r="C6" s="7">
         <v>35.259300000000003</v>
       </c>
@@ -2834,98 +3539,98 @@
       <c r="G6">
         <v>0.21132500000000001</v>
       </c>
-      <c r="H6" s="32">
+      <c r="H6" s="23">
         <f t="shared" si="0"/>
         <v>28.176666666666669</v>
       </c>
-      <c r="I6" s="23">
+      <c r="I6" s="21">
         <v>0.84282800000000002</v>
       </c>
-      <c r="J6" s="19">
+      <c r="J6" s="17">
         <v>0.15717200000000001</v>
       </c>
-      <c r="K6" s="23">
+      <c r="K6" s="21">
         <v>18230</v>
       </c>
-      <c r="L6" s="19">
+      <c r="L6" s="17">
         <v>1532</v>
       </c>
-      <c r="M6" s="19">
+      <c r="M6" s="17">
         <f t="shared" ref="M6:M11" si="1">K6+L6</f>
         <v>19762</v>
       </c>
-      <c r="N6" s="23">
+      <c r="N6" s="21">
         <v>252100</v>
       </c>
-      <c r="O6" s="19">
+      <c r="O6" s="17">
         <v>224100</v>
       </c>
-      <c r="P6" s="19">
+      <c r="P6" s="17">
         <f t="shared" ref="P6:P11" si="2">N6+O6</f>
         <v>476200</v>
       </c>
-      <c r="Q6" s="23">
+      <c r="Q6" s="21">
         <v>117.6</v>
       </c>
-      <c r="R6" s="19">
+      <c r="R6" s="17">
         <v>100.1</v>
       </c>
-      <c r="S6" s="19">
+      <c r="S6" s="17">
         <f t="shared" ref="S6:S11" si="3">Q6+R6</f>
         <v>217.7</v>
       </c>
-      <c r="T6" s="23">
+      <c r="T6" s="21">
         <v>2.08</v>
       </c>
-      <c r="U6" s="19">
+      <c r="U6" s="17">
         <v>2.5310000000000001</v>
       </c>
-      <c r="V6" s="19">
+      <c r="V6" s="17">
         <f t="shared" ref="V6:V11" si="4">T6+U6</f>
         <v>4.6110000000000007</v>
       </c>
-      <c r="W6" s="23">
+      <c r="W6" s="21">
         <v>9.1579999999999995E-2</v>
       </c>
-      <c r="X6" s="19">
+      <c r="X6" s="17">
         <v>0.1072</v>
       </c>
-      <c r="Y6" s="19">
+      <c r="Y6" s="17">
         <f t="shared" ref="Y6:Y11" si="5">W6+X6</f>
         <v>0.19878000000000001</v>
       </c>
-      <c r="Z6" s="23">
+      <c r="Z6" s="21">
         <f t="shared" ref="Z6:Z11" si="6">Q6+T6+W6</f>
         <v>119.77157999999999</v>
       </c>
-      <c r="AA6" s="19">
+      <c r="AA6" s="17">
         <f t="shared" ref="AA6:AA11" si="7">R6+U6+X6</f>
         <v>102.73820000000001</v>
       </c>
-      <c r="AB6" s="19">
+      <c r="AB6" s="17">
         <f t="shared" ref="AB6:AB11" si="8">Z6+AA6</f>
         <v>222.50977999999998</v>
       </c>
-      <c r="AC6" s="23">
+      <c r="AC6" s="21">
         <f t="shared" ref="AC6:AE11" si="9">Q6/Z6</f>
         <v>0.98186898761793084</v>
       </c>
-      <c r="AD6" s="30">
+      <c r="AD6" s="17">
         <f t="shared" si="9"/>
         <v>0.9743211385833116</v>
       </c>
-      <c r="AE6" s="30">
+      <c r="AE6" s="17">
         <f t="shared" si="9"/>
         <v>0.97838396137014749</v>
       </c>
-      <c r="AG6" s="35">
+      <c r="AG6" s="25">
         <f>4.77*222.50978*7</f>
         <v>7429.6015541999986</v>
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A7" s="25"/>
-      <c r="B7" s="26"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="29"/>
       <c r="C7" s="7">
         <v>352.59300000000002</v>
       </c>
@@ -2941,94 +3646,94 @@
       <c r="G7">
         <v>0.15699299999999999</v>
       </c>
-      <c r="H7" s="32">
+      <c r="H7" s="23">
         <f t="shared" si="0"/>
         <v>20.932400000000001</v>
       </c>
-      <c r="I7" s="23">
+      <c r="I7" s="21">
         <v>0.79603299999999999</v>
       </c>
-      <c r="J7" s="19">
+      <c r="J7" s="17">
         <v>0.20396700000000001</v>
       </c>
-      <c r="K7" s="23">
+      <c r="K7" s="21">
         <v>14010</v>
       </c>
-      <c r="L7" s="19">
+      <c r="L7" s="17">
         <v>1078</v>
       </c>
-      <c r="M7" s="19">
+      <c r="M7" s="17">
         <f t="shared" si="1"/>
         <v>15088</v>
       </c>
-      <c r="N7" s="23">
+      <c r="N7" s="21">
         <v>250600</v>
       </c>
-      <c r="O7" s="19">
+      <c r="O7" s="17">
         <v>223200</v>
       </c>
-      <c r="P7" s="19">
+      <c r="P7" s="17">
         <f t="shared" si="2"/>
         <v>473800</v>
       </c>
-      <c r="Q7" s="23">
+      <c r="Q7" s="21">
         <v>893.3</v>
       </c>
-      <c r="R7" s="19">
+      <c r="R7" s="17">
         <v>576.79999999999995</v>
       </c>
-      <c r="S7" s="19">
+      <c r="S7" s="17">
         <f t="shared" si="3"/>
         <v>1470.1</v>
       </c>
-      <c r="T7" s="23">
+      <c r="T7" s="21">
         <v>122.3</v>
       </c>
-      <c r="U7" s="19">
+      <c r="U7" s="17">
         <v>103.5</v>
       </c>
-      <c r="V7" s="19">
+      <c r="V7" s="17">
         <f t="shared" si="4"/>
         <v>225.8</v>
       </c>
-      <c r="W7" s="23">
+      <c r="W7" s="21">
         <v>56.26</v>
       </c>
-      <c r="X7" s="19">
+      <c r="X7" s="17">
         <v>35.72</v>
       </c>
-      <c r="Y7" s="19">
+      <c r="Y7" s="17">
         <f t="shared" si="5"/>
         <v>91.97999999999999</v>
       </c>
-      <c r="Z7" s="23">
+      <c r="Z7" s="21">
         <f t="shared" si="6"/>
         <v>1071.8599999999999</v>
       </c>
-      <c r="AA7" s="19">
+      <c r="AA7" s="17">
         <f t="shared" si="7"/>
         <v>716.02</v>
       </c>
-      <c r="AB7" s="19">
+      <c r="AB7" s="17">
         <f t="shared" si="8"/>
         <v>1787.8799999999999</v>
       </c>
-      <c r="AC7" s="23">
+      <c r="AC7" s="21">
         <f t="shared" si="9"/>
         <v>0.83341107980519846</v>
       </c>
-      <c r="AD7" s="30">
+      <c r="AD7" s="17">
         <f t="shared" si="9"/>
         <v>0.8055640903885366</v>
       </c>
-      <c r="AE7" s="30">
+      <c r="AE7" s="17">
         <f t="shared" si="9"/>
         <v>0.82225876457032909</v>
       </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A8" s="25"/>
-      <c r="B8" s="26"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="29"/>
       <c r="C8" s="7">
         <v>705.18499999999995</v>
       </c>
@@ -3044,94 +3749,94 @@
       <c r="G8">
         <v>9.6804000000000001E-2</v>
       </c>
-      <c r="H8" s="32">
+      <c r="H8" s="23">
         <f t="shared" si="0"/>
         <v>12.907200000000001</v>
       </c>
-      <c r="I8" s="23">
+      <c r="I8" s="21">
         <v>0.76228899999999999</v>
       </c>
-      <c r="J8" s="19">
+      <c r="J8" s="17">
         <v>0.23771100000000001</v>
       </c>
-      <c r="K8" s="23">
+      <c r="K8" s="21">
         <v>10220</v>
       </c>
-      <c r="L8" s="19">
+      <c r="L8" s="17">
         <v>720.4</v>
       </c>
-      <c r="M8" s="19">
+      <c r="M8" s="17">
         <f t="shared" si="1"/>
         <v>10940.4</v>
       </c>
-      <c r="N8" s="23">
+      <c r="N8" s="21">
         <v>248800</v>
       </c>
-      <c r="O8" s="19">
+      <c r="O8" s="17">
         <v>221900</v>
       </c>
-      <c r="P8" s="19">
+      <c r="P8" s="17">
         <f t="shared" si="2"/>
         <v>470700</v>
       </c>
-      <c r="Q8" s="23">
+      <c r="Q8" s="21">
         <v>1315</v>
       </c>
-      <c r="R8" s="19">
+      <c r="R8" s="17">
         <v>837.7</v>
       </c>
-      <c r="S8" s="19">
+      <c r="S8" s="17">
         <f t="shared" si="3"/>
         <v>2152.6999999999998</v>
       </c>
-      <c r="T8" s="23">
+      <c r="T8" s="21">
         <v>291</v>
       </c>
-      <c r="U8" s="19">
+      <c r="U8" s="17">
         <v>240.4</v>
       </c>
-      <c r="V8" s="19">
+      <c r="V8" s="17">
         <f t="shared" si="4"/>
         <v>531.4</v>
       </c>
-      <c r="W8" s="23">
+      <c r="W8" s="21">
         <v>201</v>
       </c>
-      <c r="X8" s="19">
+      <c r="X8" s="17">
         <v>124.9</v>
       </c>
-      <c r="Y8" s="19">
+      <c r="Y8" s="17">
         <f t="shared" si="5"/>
         <v>325.89999999999998</v>
       </c>
-      <c r="Z8" s="23">
+      <c r="Z8" s="21">
         <f t="shared" si="6"/>
         <v>1807</v>
       </c>
-      <c r="AA8" s="19">
+      <c r="AA8" s="17">
         <f t="shared" si="7"/>
         <v>1203.0000000000002</v>
       </c>
-      <c r="AB8" s="19">
+      <c r="AB8" s="17">
         <f t="shared" si="8"/>
         <v>3010</v>
       </c>
-      <c r="AC8" s="23">
+      <c r="AC8" s="21">
         <f t="shared" si="9"/>
         <v>0.7277255118981738</v>
       </c>
-      <c r="AD8" s="30">
+      <c r="AD8" s="17">
         <f t="shared" si="9"/>
         <v>0.69634247714048203</v>
       </c>
-      <c r="AE8" s="30">
+      <c r="AE8" s="17">
         <f t="shared" si="9"/>
         <v>0.71518272425249163</v>
       </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A9" s="25"/>
-      <c r="B9" s="26"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="29"/>
       <c r="C9" s="7">
         <v>1057.78</v>
       </c>
@@ -3147,94 +3852,94 @@
       <c r="G9">
         <v>3.4423000000000002E-2</v>
       </c>
-      <c r="H9" s="32">
+      <c r="H9" s="23">
         <f t="shared" si="0"/>
         <v>4.5897333333333341</v>
       </c>
-      <c r="I9" s="23">
+      <c r="I9" s="21">
         <v>0.73345199999999999</v>
       </c>
-      <c r="J9" s="19">
+      <c r="J9" s="17">
         <v>0.26654800000000001</v>
       </c>
-      <c r="K9" s="23">
+      <c r="K9" s="21">
         <v>7165</v>
       </c>
-      <c r="L9" s="19">
+      <c r="L9" s="17">
         <v>473.9</v>
       </c>
-      <c r="M9" s="19">
+      <c r="M9" s="17">
         <f t="shared" si="1"/>
         <v>7638.9</v>
       </c>
-      <c r="N9" s="23">
+      <c r="N9" s="21">
         <v>246800</v>
       </c>
-      <c r="O9" s="19">
+      <c r="O9" s="17">
         <v>220500</v>
       </c>
-      <c r="P9" s="19">
+      <c r="P9" s="17">
         <f t="shared" si="2"/>
         <v>467300</v>
       </c>
-      <c r="Q9" s="23">
+      <c r="Q9" s="21">
         <v>1503</v>
       </c>
-      <c r="R9" s="19">
+      <c r="R9" s="17">
         <v>975.7</v>
       </c>
-      <c r="S9" s="19">
+      <c r="S9" s="17">
         <f t="shared" si="3"/>
         <v>2478.6999999999998</v>
       </c>
-      <c r="T9" s="23">
+      <c r="T9" s="21">
         <v>457.8</v>
       </c>
-      <c r="U9" s="19">
+      <c r="U9" s="17">
         <v>366</v>
       </c>
-      <c r="V9" s="19">
+      <c r="V9" s="17">
         <f t="shared" si="4"/>
         <v>823.8</v>
       </c>
-      <c r="W9" s="23">
+      <c r="W9" s="21">
         <v>334.8</v>
       </c>
-      <c r="X9" s="19">
+      <c r="X9" s="17">
         <v>206.4</v>
       </c>
-      <c r="Y9" s="19">
+      <c r="Y9" s="17">
         <f t="shared" si="5"/>
         <v>541.20000000000005</v>
       </c>
-      <c r="Z9" s="23">
+      <c r="Z9" s="21">
         <f t="shared" si="6"/>
         <v>2295.6</v>
       </c>
-      <c r="AA9" s="19">
+      <c r="AA9" s="17">
         <f t="shared" si="7"/>
         <v>1548.1000000000001</v>
       </c>
-      <c r="AB9" s="19">
+      <c r="AB9" s="17">
         <f t="shared" si="8"/>
         <v>3843.7</v>
       </c>
-      <c r="AC9" s="23">
+      <c r="AC9" s="21">
         <f t="shared" si="9"/>
         <v>0.65473078933612128</v>
       </c>
-      <c r="AD9" s="30">
+      <c r="AD9" s="17">
         <f t="shared" si="9"/>
         <v>0.63025644338221043</v>
       </c>
-      <c r="AE9" s="30">
+      <c r="AE9" s="17">
         <f t="shared" si="9"/>
         <v>0.64487342924786006</v>
       </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A10" s="25"/>
-      <c r="B10" s="26"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="29"/>
       <c r="C10" s="7">
         <v>1410.37</v>
       </c>
@@ -3250,205 +3955,205 @@
       <c r="G10">
         <v>-3.2662999999999998E-2</v>
       </c>
-      <c r="H10" s="32">
+      <c r="H10" s="23">
         <f t="shared" si="0"/>
         <v>-4.3550666666666666</v>
       </c>
-      <c r="I10" s="23">
+      <c r="I10" s="21">
         <v>0.70491000000000004</v>
       </c>
-      <c r="J10" s="19">
+      <c r="J10" s="17">
         <v>0.29509000000000002</v>
       </c>
-      <c r="K10" s="23">
+      <c r="K10" s="21">
         <v>4755</v>
       </c>
-      <c r="L10" s="19">
+      <c r="L10" s="17">
         <v>304.8</v>
       </c>
-      <c r="M10" s="19">
+      <c r="M10" s="17">
         <f t="shared" si="1"/>
         <v>5059.8</v>
       </c>
-      <c r="N10" s="23">
+      <c r="N10" s="21">
         <v>244600</v>
       </c>
-      <c r="O10" s="19">
+      <c r="O10" s="17">
         <v>218900</v>
       </c>
-      <c r="P10" s="19">
+      <c r="P10" s="17">
         <f t="shared" si="2"/>
         <v>463500</v>
       </c>
-      <c r="Q10" s="23">
+      <c r="Q10" s="21">
         <v>1555</v>
       </c>
-      <c r="R10" s="19">
+      <c r="R10" s="17">
         <v>1052</v>
       </c>
-      <c r="S10" s="19">
+      <c r="S10" s="17">
         <f t="shared" si="3"/>
         <v>2607</v>
       </c>
-      <c r="T10" s="23">
+      <c r="T10" s="21">
         <v>605.20000000000005</v>
       </c>
-      <c r="U10" s="19">
+      <c r="U10" s="17">
         <v>472.7</v>
       </c>
-      <c r="V10" s="19">
+      <c r="V10" s="17">
         <f t="shared" si="4"/>
         <v>1077.9000000000001</v>
       </c>
-      <c r="W10" s="23">
+      <c r="W10" s="21">
         <v>429.9</v>
       </c>
-      <c r="X10" s="19">
+      <c r="X10" s="17">
         <v>269.39999999999998</v>
       </c>
-      <c r="Y10" s="19">
+      <c r="Y10" s="17">
         <f t="shared" si="5"/>
         <v>699.3</v>
       </c>
-      <c r="Z10" s="23">
+      <c r="Z10" s="21">
         <f t="shared" si="6"/>
         <v>2590.1</v>
       </c>
-      <c r="AA10" s="19">
+      <c r="AA10" s="17">
         <f t="shared" si="7"/>
         <v>1794.1</v>
       </c>
-      <c r="AB10" s="19">
+      <c r="AB10" s="17">
         <f t="shared" si="8"/>
         <v>4384.2</v>
       </c>
-      <c r="AC10" s="23">
+      <c r="AC10" s="21">
         <f t="shared" si="9"/>
         <v>0.6003629203505656</v>
       </c>
-      <c r="AD10" s="30">
+      <c r="AD10" s="17">
         <f t="shared" si="9"/>
         <v>0.58636642327629451</v>
       </c>
-      <c r="AE10" s="30">
+      <c r="AE10" s="17">
         <f t="shared" si="9"/>
         <v>0.59463528123716991</v>
       </c>
     </row>
-    <row r="11" spans="1:33" s="20" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="27"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="22">
+    <row r="11" spans="1:33" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="30"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="20">
         <v>1762.96</v>
       </c>
-      <c r="D11" s="20">
+      <c r="D11" s="18">
         <v>50</v>
       </c>
-      <c r="E11" s="20">
+      <c r="E11" s="18">
         <v>0.90683000000000002</v>
       </c>
-      <c r="F11" s="20">
+      <c r="F11" s="18">
         <v>2.1000000000000001E-4</v>
       </c>
-      <c r="G11" s="20">
+      <c r="G11" s="18">
         <v>-0.102743</v>
       </c>
-      <c r="H11" s="33">
+      <c r="H11" s="24">
         <f t="shared" si="0"/>
         <v>-13.699066666666667</v>
       </c>
-      <c r="I11" s="24">
+      <c r="I11" s="22">
         <v>0.67607200000000001</v>
       </c>
-      <c r="J11" s="21">
+      <c r="J11" s="19">
         <v>0.32392799999999999</v>
       </c>
-      <c r="K11" s="24">
+      <c r="K11" s="22">
         <v>2954</v>
       </c>
-      <c r="L11" s="21">
+      <c r="L11" s="19">
         <v>190.3</v>
       </c>
-      <c r="M11" s="21">
+      <c r="M11" s="19">
         <f t="shared" si="1"/>
         <v>3144.3</v>
       </c>
-      <c r="N11" s="24">
+      <c r="N11" s="22">
         <v>242200</v>
       </c>
-      <c r="O11" s="21">
+      <c r="O11" s="19">
         <v>217300</v>
       </c>
-      <c r="P11" s="21">
+      <c r="P11" s="19">
         <f t="shared" si="2"/>
         <v>459500</v>
       </c>
-      <c r="Q11" s="24">
+      <c r="Q11" s="22">
         <v>1536</v>
       </c>
-      <c r="R11" s="21">
+      <c r="R11" s="19">
         <v>1094</v>
       </c>
-      <c r="S11" s="21">
+      <c r="S11" s="19">
         <f t="shared" si="3"/>
         <v>2630</v>
       </c>
-      <c r="T11" s="24">
+      <c r="T11" s="22">
         <v>721</v>
       </c>
-      <c r="U11" s="21">
+      <c r="U11" s="19">
         <v>559.5</v>
       </c>
-      <c r="V11" s="21">
+      <c r="V11" s="19">
         <f t="shared" si="4"/>
         <v>1280.5</v>
       </c>
-      <c r="W11" s="24">
+      <c r="W11" s="22">
         <v>486</v>
       </c>
-      <c r="X11" s="21">
+      <c r="X11" s="19">
         <v>315.89999999999998</v>
       </c>
-      <c r="Y11" s="21">
+      <c r="Y11" s="19">
         <f t="shared" si="5"/>
         <v>801.9</v>
       </c>
-      <c r="Z11" s="24">
+      <c r="Z11" s="22">
         <f t="shared" si="6"/>
         <v>2743</v>
       </c>
-      <c r="AA11" s="21">
+      <c r="AA11" s="19">
         <f t="shared" si="7"/>
         <v>1969.4</v>
       </c>
-      <c r="AB11" s="21">
+      <c r="AB11" s="19">
         <f t="shared" si="8"/>
         <v>4712.3999999999996</v>
       </c>
-      <c r="AC11" s="24">
+      <c r="AC11" s="22">
         <f t="shared" si="9"/>
         <v>0.55997083485235144</v>
       </c>
-      <c r="AD11" s="21">
+      <c r="AD11" s="19">
         <f t="shared" si="9"/>
         <v>0.55549913679293184</v>
       </c>
-      <c r="AE11" s="21">
+      <c r="AE11" s="19">
         <f t="shared" si="9"/>
         <v>0.55810202869026404</v>
       </c>
     </row>
-    <row r="12" spans="1:33" s="20" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="22"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="22"/>
-      <c r="N12" s="22"/>
-      <c r="Q12" s="22"/>
-      <c r="T12" s="22"/>
-      <c r="W12" s="22"/>
-      <c r="Z12" s="22"/>
-      <c r="AC12" s="22"/>
+    <row r="12" spans="1:33" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="20"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="20"/>
+      <c r="N12" s="20"/>
+      <c r="Q12" s="20"/>
+      <c r="T12" s="20"/>
+      <c r="W12" s="20"/>
+      <c r="Z12" s="20"/>
+      <c r="AC12" s="20"/>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
@@ -3574,10 +4279,10 @@
       <c r="AC14" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="AD14" s="29" t="s">
+      <c r="AD14" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AE14" s="29" t="s">
+      <c r="AE14" s="1" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3603,23 +4308,23 @@
       <c r="G15">
         <v>0.18729599999999999</v>
       </c>
-      <c r="H15" s="32">
+      <c r="H15" s="23">
         <f>G15/0.0075</f>
         <v>24.972799999999999</v>
       </c>
-      <c r="I15" s="23">
+      <c r="I15" s="21">
         <v>0.63836199999999999</v>
       </c>
-      <c r="J15" s="19">
+      <c r="J15" s="17">
         <v>0.36163800000000001</v>
       </c>
       <c r="Z15" s="7">
         <v>0</v>
       </c>
-      <c r="AA15" s="31">
+      <c r="AA15">
         <v>0</v>
       </c>
-      <c r="AB15" s="31">
+      <c r="AB15">
         <v>0</v>
       </c>
     </row>
@@ -3645,87 +4350,87 @@
       <c r="G16">
         <v>0.16094</v>
       </c>
-      <c r="H16" s="32">
+      <c r="H16" s="23">
         <f t="shared" ref="H16:H22" si="10">G16/0.0075</f>
         <v>21.458666666666666</v>
       </c>
-      <c r="I16" s="23">
+      <c r="I16" s="21">
         <v>0.634965</v>
       </c>
-      <c r="J16" s="19">
+      <c r="J16" s="17">
         <v>0.365035</v>
       </c>
-      <c r="K16" s="23">
+      <c r="K16" s="21">
         <v>14020</v>
       </c>
-      <c r="L16" s="19">
+      <c r="L16" s="17">
         <v>2069</v>
       </c>
-      <c r="M16" s="19">
+      <c r="M16" s="17">
         <f>K16+L16</f>
         <v>16089</v>
       </c>
-      <c r="N16" s="23">
+      <c r="N16" s="21">
         <v>189200</v>
       </c>
-      <c r="O16" s="19">
+      <c r="O16" s="17">
         <v>291500</v>
       </c>
-      <c r="P16" s="19">
+      <c r="P16" s="17">
         <f>N16+O16</f>
         <v>480700</v>
       </c>
-      <c r="Q16" s="23">
+      <c r="Q16" s="21">
         <v>3.5760000000000001</v>
       </c>
-      <c r="R16" s="19">
+      <c r="R16" s="17">
         <v>10.199999999999999</v>
       </c>
-      <c r="S16" s="19">
+      <c r="S16" s="17">
         <f>Q16+R16</f>
         <v>13.776</v>
       </c>
-      <c r="T16" s="23">
+      <c r="T16" s="21">
         <v>1.0059999999999999E-2</v>
       </c>
-      <c r="U16" s="19">
+      <c r="U16" s="17">
         <v>6.6710000000000005E-2</v>
       </c>
-      <c r="V16" s="19">
+      <c r="V16" s="17">
         <f>T16+U16</f>
         <v>7.6770000000000005E-2</v>
       </c>
-      <c r="W16" s="23">
+      <c r="W16" s="21">
         <v>9.9599999999999995E-6</v>
       </c>
-      <c r="X16" s="19">
+      <c r="X16" s="17">
         <v>4.7029999999999999E-4</v>
       </c>
-      <c r="Y16" s="19">
+      <c r="Y16" s="17">
         <f>W16+X16</f>
         <v>4.8025999999999999E-4</v>
       </c>
-      <c r="Z16" s="23">
+      <c r="Z16" s="21">
         <f>Q16+T16+W16</f>
         <v>3.5860699600000001</v>
       </c>
-      <c r="AA16" s="19">
+      <c r="AA16" s="17">
         <f>R16+U16+X16</f>
         <v>10.2671803</v>
       </c>
-      <c r="AB16" s="19">
+      <c r="AB16" s="17">
         <f>Z16+AA16</f>
         <v>13.853250259999999</v>
       </c>
-      <c r="AC16" s="23">
+      <c r="AC16" s="21">
         <f>Q16/Z16</f>
         <v>0.99719192316036132</v>
       </c>
-      <c r="AD16" s="30">
+      <c r="AD16" s="17">
         <f>R16/AA16</f>
         <v>0.99345679163733003</v>
       </c>
-      <c r="AE16" s="30">
+      <c r="AE16" s="17">
         <f>S16/AB16</f>
         <v>0.99442367252809594</v>
       </c>
@@ -3734,10 +4439,10 @@
       </c>
     </row>
     <row r="17" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="A17" s="25" t="e" vm="1">
+      <c r="A17" s="28" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
-      <c r="B17" s="26"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="7">
         <v>35.259300000000003</v>
       </c>
@@ -3753,91 +4458,91 @@
       <c r="G17">
         <v>0.15795899999999999</v>
       </c>
-      <c r="H17" s="32">
+      <c r="H17" s="23">
         <f t="shared" si="10"/>
         <v>21.061199999999999</v>
       </c>
-      <c r="I17" s="23">
+      <c r="I17" s="21">
         <v>0.61049100000000001</v>
       </c>
-      <c r="J17" s="19">
+      <c r="J17" s="17">
         <v>0.38950899999999999</v>
       </c>
-      <c r="K17" s="23">
+      <c r="K17" s="21">
         <v>13670</v>
       </c>
-      <c r="L17" s="19">
+      <c r="L17" s="17">
         <v>1907</v>
       </c>
-      <c r="M17" s="19">
+      <c r="M17" s="17">
         <f t="shared" ref="M17:M22" si="11">K17+L17</f>
         <v>15577</v>
       </c>
-      <c r="N17" s="23">
+      <c r="N17" s="21">
         <v>189100</v>
       </c>
-      <c r="O17" s="19">
+      <c r="O17" s="17">
         <v>291200</v>
       </c>
-      <c r="P17" s="19">
+      <c r="P17" s="17">
         <f t="shared" ref="P17:P22" si="12">N17+O17</f>
         <v>480300</v>
       </c>
-      <c r="Q17" s="23">
+      <c r="Q17" s="21">
         <v>84.6</v>
       </c>
-      <c r="R17" s="19">
+      <c r="R17" s="17">
         <v>210.4</v>
       </c>
-      <c r="S17" s="19">
+      <c r="S17" s="17">
         <f t="shared" ref="S17:S22" si="13">Q17+R17</f>
         <v>295</v>
       </c>
-      <c r="T17" s="23">
+      <c r="T17" s="21">
         <v>1.474</v>
       </c>
-      <c r="U17" s="19">
+      <c r="U17" s="17">
         <v>9.7750000000000004</v>
       </c>
-      <c r="V17" s="19">
+      <c r="V17" s="17">
         <f t="shared" ref="V17:V22" si="14">T17+U17</f>
         <v>11.249000000000001</v>
       </c>
-      <c r="W17" s="23">
+      <c r="W17" s="21">
         <v>6.173E-2</v>
       </c>
-      <c r="X17" s="19">
+      <c r="X17" s="17">
         <v>8.0299999999999996E-2</v>
       </c>
-      <c r="Y17" s="19">
+      <c r="Y17" s="17">
         <f t="shared" ref="Y17:Y22" si="15">W17+X17</f>
         <v>0.14202999999999999</v>
       </c>
-      <c r="Z17" s="23">
+      <c r="Z17" s="21">
         <f t="shared" ref="Z17:Z22" si="16">Q17+T17+W17</f>
         <v>86.135729999999995</v>
       </c>
-      <c r="AA17" s="19">
+      <c r="AA17" s="17">
         <f t="shared" ref="AA17:AA22" si="17">R17+U17+X17</f>
         <v>220.25530000000001</v>
       </c>
-      <c r="AB17" s="19">
+      <c r="AB17" s="17">
         <f t="shared" ref="AB17:AB22" si="18">Z17+AA17</f>
         <v>306.39103</v>
       </c>
-      <c r="AC17" s="23">
+      <c r="AC17" s="21">
         <f t="shared" ref="AC17:AC22" si="19">Q17/Z17</f>
         <v>0.98217081343595736</v>
       </c>
-      <c r="AD17" s="30">
+      <c r="AD17" s="17">
         <f t="shared" ref="AD17:AD22" si="20">R17/AA17</f>
         <v>0.95525510623353904</v>
       </c>
-      <c r="AE17" s="30">
+      <c r="AE17" s="17">
         <f t="shared" ref="AE17:AE22" si="21">S17/AB17</f>
         <v>0.96282192073312334</v>
       </c>
-      <c r="AG17" s="35">
+      <c r="AG17" s="25">
         <f>4.77*306.39103*7</f>
         <v>10230.396491699998</v>
       </c>
@@ -3846,8 +4551,8 @@
       </c>
     </row>
     <row r="18" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="A18" s="25"/>
-      <c r="B18" s="26"/>
+      <c r="A18" s="28"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="7">
         <v>352.59300000000002</v>
       </c>
@@ -3863,94 +4568,94 @@
       <c r="G18">
         <v>0.103935</v>
       </c>
-      <c r="H18" s="32">
+      <c r="H18" s="23">
         <f t="shared" si="10"/>
         <v>13.858000000000001</v>
       </c>
-      <c r="I18" s="23">
+      <c r="I18" s="21">
         <v>0.54753300000000005</v>
       </c>
-      <c r="J18" s="19">
+      <c r="J18" s="17">
         <v>0.45246700000000001</v>
       </c>
-      <c r="K18" s="23">
+      <c r="K18" s="21">
         <v>10610</v>
       </c>
-      <c r="L18" s="19">
+      <c r="L18" s="17">
         <v>1002</v>
       </c>
-      <c r="M18" s="19">
+      <c r="M18" s="17">
         <f t="shared" si="11"/>
         <v>11612</v>
       </c>
-      <c r="N18" s="23">
+      <c r="N18" s="21">
         <v>188000</v>
       </c>
-      <c r="O18" s="19">
+      <c r="O18" s="17">
         <v>289100</v>
       </c>
-      <c r="P18" s="19">
+      <c r="P18" s="17">
         <f t="shared" si="12"/>
         <v>477100</v>
       </c>
-      <c r="Q18" s="23">
+      <c r="Q18" s="21">
         <v>641.79999999999995</v>
       </c>
-      <c r="R18" s="19">
+      <c r="R18" s="17">
         <v>878.8</v>
       </c>
-      <c r="S18" s="19">
+      <c r="S18" s="17">
         <f t="shared" si="13"/>
         <v>1520.6</v>
       </c>
-      <c r="T18" s="23">
+      <c r="T18" s="21">
         <v>86.36</v>
       </c>
-      <c r="U18" s="19">
+      <c r="U18" s="17">
         <v>250.7</v>
       </c>
-      <c r="V18" s="19">
+      <c r="V18" s="17">
         <f t="shared" si="14"/>
         <v>337.06</v>
       </c>
-      <c r="W18" s="23">
+      <c r="W18" s="21">
         <v>37.18</v>
       </c>
-      <c r="X18" s="19">
+      <c r="X18" s="17">
         <v>124.9</v>
       </c>
-      <c r="Y18" s="19">
+      <c r="Y18" s="17">
         <f t="shared" si="15"/>
         <v>162.08000000000001</v>
       </c>
-      <c r="Z18" s="23">
+      <c r="Z18" s="21">
         <f t="shared" si="16"/>
         <v>765.33999999999992</v>
       </c>
-      <c r="AA18" s="19">
+      <c r="AA18" s="17">
         <f t="shared" si="17"/>
         <v>1254.4000000000001</v>
       </c>
-      <c r="AB18" s="19">
+      <c r="AB18" s="17">
         <f t="shared" si="18"/>
         <v>2019.74</v>
       </c>
-      <c r="AC18" s="23">
+      <c r="AC18" s="21">
         <f t="shared" si="19"/>
         <v>0.8385815454569211</v>
       </c>
-      <c r="AD18" s="30">
+      <c r="AD18" s="17">
         <f t="shared" si="20"/>
         <v>0.70057397959183665</v>
       </c>
-      <c r="AE18" s="30">
+      <c r="AE18" s="17">
         <f t="shared" si="21"/>
         <v>0.75286918118173618</v>
       </c>
     </row>
     <row r="19" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="A19" s="25"/>
-      <c r="B19" s="26"/>
+      <c r="A19" s="28"/>
+      <c r="B19" s="29"/>
       <c r="C19" s="7">
         <v>705.18499999999995</v>
       </c>
@@ -3966,94 +4671,94 @@
       <c r="G19">
         <v>4.5419000000000001E-2</v>
       </c>
-      <c r="H19" s="32">
+      <c r="H19" s="23">
         <f t="shared" si="10"/>
         <v>6.0558666666666667</v>
       </c>
-      <c r="I19" s="23">
+      <c r="I19" s="21">
         <v>0.51253000000000004</v>
       </c>
-      <c r="J19" s="19">
+      <c r="J19" s="17">
         <v>0.48747000000000001</v>
       </c>
-      <c r="K19" s="23">
+      <c r="K19" s="21">
         <v>7969</v>
       </c>
-      <c r="L19" s="19">
+      <c r="L19" s="17">
         <v>503.3</v>
       </c>
-      <c r="M19" s="19">
+      <c r="M19" s="17">
         <f t="shared" si="11"/>
         <v>8472.2999999999993</v>
       </c>
-      <c r="N19" s="23">
+      <c r="N19" s="21">
         <v>186800</v>
       </c>
-      <c r="O19" s="19">
+      <c r="O19" s="17">
         <v>286500</v>
       </c>
-      <c r="P19" s="19">
+      <c r="P19" s="17">
         <f t="shared" si="12"/>
         <v>473300</v>
       </c>
-      <c r="Q19" s="23">
+      <c r="Q19" s="21">
         <v>951.8</v>
       </c>
-      <c r="R19" s="19">
+      <c r="R19" s="17">
         <v>1143</v>
       </c>
-      <c r="S19" s="19">
+      <c r="S19" s="17">
         <f t="shared" si="13"/>
         <v>2094.8000000000002</v>
       </c>
-      <c r="T19" s="23">
+      <c r="T19" s="21">
         <v>203.8</v>
       </c>
-      <c r="U19" s="19">
+      <c r="U19" s="17">
         <v>478.7</v>
       </c>
-      <c r="V19" s="19">
+      <c r="V19" s="17">
         <f t="shared" si="14"/>
         <v>682.5</v>
       </c>
-      <c r="W19" s="23">
+      <c r="W19" s="21">
         <v>131.5</v>
       </c>
-      <c r="X19" s="19">
+      <c r="X19" s="17">
         <v>272.10000000000002</v>
       </c>
-      <c r="Y19" s="19">
+      <c r="Y19" s="17">
         <f t="shared" si="15"/>
         <v>403.6</v>
       </c>
-      <c r="Z19" s="23">
+      <c r="Z19" s="21">
         <f t="shared" si="16"/>
         <v>1287.0999999999999</v>
       </c>
-      <c r="AA19" s="19">
+      <c r="AA19" s="17">
         <f t="shared" si="17"/>
         <v>1893.8000000000002</v>
       </c>
-      <c r="AB19" s="19">
+      <c r="AB19" s="17">
         <f t="shared" si="18"/>
         <v>3180.9</v>
       </c>
-      <c r="AC19" s="23">
+      <c r="AC19" s="21">
         <f t="shared" si="19"/>
         <v>0.73949188097272944</v>
       </c>
-      <c r="AD19" s="30">
+      <c r="AD19" s="17">
         <f t="shared" si="20"/>
         <v>0.60354842116379759</v>
       </c>
-      <c r="AE19" s="30">
+      <c r="AE19" s="17">
         <f t="shared" si="21"/>
         <v>0.65855575466063065</v>
       </c>
     </row>
     <row r="20" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="A20" s="25"/>
-      <c r="B20" s="26"/>
+      <c r="A20" s="28"/>
+      <c r="B20" s="29"/>
       <c r="C20" s="7">
         <v>1057.78</v>
       </c>
@@ -4069,94 +4774,94 @@
       <c r="G20">
         <v>-1.2381E-2</v>
       </c>
-      <c r="H20" s="32">
+      <c r="H20" s="23">
         <f t="shared" si="10"/>
         <v>-1.6508</v>
       </c>
-      <c r="I20" s="23">
+      <c r="I20" s="21">
         <v>0.484315</v>
       </c>
-      <c r="J20" s="19">
+      <c r="J20" s="17">
         <v>0.51568499999999995</v>
       </c>
-      <c r="K20" s="23">
+      <c r="K20" s="21">
         <v>5843</v>
       </c>
-      <c r="L20" s="19">
+      <c r="L20" s="17">
         <v>255.6</v>
       </c>
-      <c r="M20" s="19">
+      <c r="M20" s="17">
         <f t="shared" si="11"/>
         <v>6098.6</v>
       </c>
-      <c r="N20" s="23">
+      <c r="N20" s="21">
         <v>185500</v>
       </c>
-      <c r="O20" s="19">
+      <c r="O20" s="17">
         <v>283700</v>
       </c>
-      <c r="P20" s="19">
+      <c r="P20" s="17">
         <f t="shared" si="12"/>
         <v>469200</v>
       </c>
-      <c r="Q20" s="23">
+      <c r="Q20" s="21">
         <v>1098</v>
       </c>
-      <c r="R20" s="19">
+      <c r="R20" s="17">
         <v>1272</v>
       </c>
-      <c r="S20" s="19">
+      <c r="S20" s="17">
         <f t="shared" si="13"/>
         <v>2370</v>
       </c>
-      <c r="T20" s="23">
+      <c r="T20" s="21">
         <v>318.2</v>
       </c>
-      <c r="U20" s="19">
+      <c r="U20" s="17">
         <v>647.20000000000005</v>
       </c>
-      <c r="V20" s="19">
+      <c r="V20" s="17">
         <f t="shared" si="14"/>
         <v>965.40000000000009</v>
       </c>
-      <c r="W20" s="23">
+      <c r="W20" s="21">
         <v>223.1</v>
       </c>
-      <c r="X20" s="19">
+      <c r="X20" s="17">
         <v>362.1</v>
       </c>
-      <c r="Y20" s="19">
+      <c r="Y20" s="17">
         <f t="shared" si="15"/>
         <v>585.20000000000005</v>
       </c>
-      <c r="Z20" s="23">
+      <c r="Z20" s="21">
         <f t="shared" si="16"/>
         <v>1639.3</v>
       </c>
-      <c r="AA20" s="19">
+      <c r="AA20" s="17">
         <f t="shared" si="17"/>
         <v>2281.3000000000002</v>
       </c>
-      <c r="AB20" s="19">
+      <c r="AB20" s="17">
         <f t="shared" si="18"/>
         <v>3920.6000000000004</v>
       </c>
-      <c r="AC20" s="23">
+      <c r="AC20" s="21">
         <f t="shared" si="19"/>
         <v>0.66979808454828282</v>
       </c>
-      <c r="AD20" s="30">
+      <c r="AD20" s="17">
         <f t="shared" si="20"/>
         <v>0.55757682023407706</v>
       </c>
-      <c r="AE20" s="30">
+      <c r="AE20" s="17">
         <f t="shared" si="21"/>
         <v>0.60449931132989843</v>
       </c>
     </row>
     <row r="21" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="A21" s="25"/>
-      <c r="B21" s="26"/>
+      <c r="A21" s="28"/>
+      <c r="B21" s="29"/>
       <c r="C21" s="7">
         <v>1410.37</v>
       </c>
@@ -4172,190 +4877,190 @@
       <c r="G21">
         <v>-6.8650000000000003E-2</v>
       </c>
-      <c r="H21" s="32">
+      <c r="H21" s="23">
         <f t="shared" si="10"/>
         <v>-9.1533333333333342</v>
       </c>
-      <c r="I21" s="23">
+      <c r="I21" s="21">
         <v>0.455762</v>
       </c>
-      <c r="J21" s="19">
+      <c r="J21" s="17">
         <v>0.544238</v>
       </c>
-      <c r="K21" s="23">
+      <c r="K21" s="21">
         <v>4146</v>
       </c>
-      <c r="L21" s="19">
+      <c r="L21" s="17">
         <v>129.80000000000001</v>
       </c>
-      <c r="M21" s="19">
+      <c r="M21" s="17">
         <f t="shared" si="11"/>
         <v>4275.8</v>
       </c>
-      <c r="N21" s="23">
+      <c r="N21" s="21">
         <v>184100</v>
       </c>
-      <c r="O21" s="19">
+      <c r="O21" s="17">
         <v>280700</v>
       </c>
-      <c r="P21" s="19">
+      <c r="P21" s="17">
         <f t="shared" si="12"/>
         <v>464800</v>
       </c>
-      <c r="Q21" s="23">
+      <c r="Q21" s="21">
         <v>1154</v>
       </c>
-      <c r="R21" s="19">
+      <c r="R21" s="17">
         <v>1347</v>
       </c>
-      <c r="S21" s="19">
+      <c r="S21" s="17">
         <f t="shared" si="13"/>
         <v>2501</v>
       </c>
-      <c r="T21" s="23">
+      <c r="T21" s="21">
         <v>421.4</v>
       </c>
-      <c r="U21" s="19">
+      <c r="U21" s="17">
         <v>765.5</v>
       </c>
-      <c r="V21" s="19">
+      <c r="V21" s="17">
         <f t="shared" si="14"/>
         <v>1186.9000000000001</v>
       </c>
-      <c r="W21" s="23">
+      <c r="W21" s="21">
         <v>292.39999999999998</v>
       </c>
-      <c r="X21" s="19">
+      <c r="X21" s="17">
         <v>421.5</v>
       </c>
-      <c r="Y21" s="19">
+      <c r="Y21" s="17">
         <f t="shared" si="15"/>
         <v>713.9</v>
       </c>
-      <c r="Z21" s="23">
+      <c r="Z21" s="21">
         <f t="shared" si="16"/>
         <v>1867.8000000000002</v>
       </c>
-      <c r="AA21" s="19">
+      <c r="AA21" s="17">
         <f t="shared" si="17"/>
         <v>2534</v>
       </c>
-      <c r="AB21" s="19">
+      <c r="AB21" s="17">
         <f t="shared" si="18"/>
         <v>4401.8</v>
       </c>
-      <c r="AC21" s="23">
+      <c r="AC21" s="21">
         <f t="shared" si="19"/>
         <v>0.61783916907591818</v>
       </c>
-      <c r="AD21" s="30">
+      <c r="AD21" s="17">
         <f t="shared" si="20"/>
         <v>0.5315706393054459</v>
       </c>
-      <c r="AE21" s="30">
+      <c r="AE21" s="17">
         <f t="shared" si="21"/>
         <v>0.56817665500477077</v>
       </c>
     </row>
-    <row r="22" spans="1:51" s="20" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="27"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="22">
+    <row r="22" spans="1:51" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="30"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="20">
         <v>1762.96</v>
       </c>
-      <c r="D22" s="20">
+      <c r="D22" s="18">
         <v>50</v>
       </c>
-      <c r="E22" s="20">
+      <c r="E22" s="18">
         <v>0.88985999999999998</v>
       </c>
-      <c r="F22" s="20">
+      <c r="F22" s="18">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="G22" s="20">
+      <c r="G22" s="18">
         <v>-0.12377199999999999</v>
       </c>
-      <c r="H22" s="33">
+      <c r="H22" s="24">
         <f t="shared" si="10"/>
         <v>-16.502933333333335</v>
       </c>
-      <c r="I22" s="24">
+      <c r="I22" s="22">
         <v>0.427315</v>
       </c>
-      <c r="J22" s="21">
+      <c r="J22" s="19">
         <v>0.572685</v>
       </c>
-      <c r="K22" s="24">
+      <c r="K22" s="22">
         <v>2836</v>
       </c>
-      <c r="L22" s="21">
+      <c r="L22" s="19">
         <v>65.459999999999994</v>
       </c>
-      <c r="M22" s="21">
+      <c r="M22" s="19">
         <f t="shared" si="11"/>
         <v>2901.46</v>
       </c>
-      <c r="N22" s="24">
+      <c r="N22" s="22">
         <v>182600</v>
       </c>
-      <c r="O22" s="21">
+      <c r="O22" s="19">
         <v>277600</v>
       </c>
-      <c r="P22" s="21">
+      <c r="P22" s="19">
         <f t="shared" si="12"/>
         <v>460200</v>
       </c>
-      <c r="Q22" s="24">
+      <c r="Q22" s="22">
         <v>1159</v>
       </c>
-      <c r="R22" s="21">
+      <c r="R22" s="19">
         <v>1396</v>
       </c>
-      <c r="S22" s="21">
+      <c r="S22" s="19">
         <f t="shared" si="13"/>
         <v>2555</v>
       </c>
-      <c r="T22" s="24">
+      <c r="T22" s="22">
         <v>7.9</v>
       </c>
-      <c r="U22" s="21">
+      <c r="U22" s="19">
         <v>847.6</v>
       </c>
-      <c r="V22" s="21">
+      <c r="V22" s="19">
         <f t="shared" si="14"/>
         <v>855.5</v>
       </c>
-      <c r="W22" s="24">
+      <c r="W22" s="22">
         <v>337.5</v>
       </c>
-      <c r="X22" s="21">
+      <c r="X22" s="19">
         <v>462.5</v>
       </c>
-      <c r="Y22" s="21">
+      <c r="Y22" s="19">
         <f t="shared" si="15"/>
         <v>800</v>
       </c>
-      <c r="Z22" s="24">
+      <c r="Z22" s="22">
         <f t="shared" si="16"/>
         <v>1504.4</v>
       </c>
-      <c r="AA22" s="21">
+      <c r="AA22" s="19">
         <f t="shared" si="17"/>
         <v>2706.1</v>
       </c>
-      <c r="AB22" s="21">
+      <c r="AB22" s="19">
         <f t="shared" si="18"/>
         <v>4210.5</v>
       </c>
-      <c r="AC22" s="24">
+      <c r="AC22" s="22">
         <f t="shared" si="19"/>
         <v>0.77040680670034556</v>
       </c>
-      <c r="AD22" s="21">
+      <c r="AD22" s="19">
         <f t="shared" si="20"/>
         <v>0.51587154946232583</v>
       </c>
-      <c r="AE22" s="21">
+      <c r="AE22" s="19">
         <f t="shared" si="21"/>
         <v>0.60681629260182879</v>
       </c>

</xml_diff>

<commit_message>
core C lithium-doped cladding
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickpark/Desktop/elwr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0919E8CD-3F47-CE46-9340-A4DCE011C3AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE9350C-0A05-2944-AA7D-D086E7872E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4368,8 +4368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E48A428C-A2D0-4C30-9161-4343E51EC6DC}">
   <dimension ref="A1:BB61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P33" zoomScale="141" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AI53" sqref="AI53"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="141" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7627,7 +7627,7 @@
         <f>R40/AD40</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AH40" s="17">
+      <c r="AH40" s="23">
         <f>S40/AE40</f>
         <v>0.99690279079407218</v>
       </c>
@@ -7723,7 +7723,7 @@
         <v>0.97897914138870401</v>
       </c>
       <c r="AG41" s="17"/>
-      <c r="AH41" s="17">
+      <c r="AH41" s="23">
         <f t="shared" ref="AH41:AH43" si="45">S41/AE41</f>
         <v>0.97897914138870401</v>
       </c>
@@ -7815,7 +7815,7 @@
         <v>0.91805727192984465</v>
       </c>
       <c r="AG42" s="17"/>
-      <c r="AH42" s="17">
+      <c r="AH42" s="23">
         <f t="shared" si="45"/>
         <v>0.91805727192984465</v>
       </c>
@@ -7910,7 +7910,7 @@
         <f t="shared" ref="AG43:AG48" si="48">R43/AD43</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AH43" s="17">
+      <c r="AH43" s="23">
         <f t="shared" si="45"/>
         <v>0.86380895283772985</v>
       </c>
@@ -8011,7 +8011,7 @@
         <f t="shared" si="48"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AH44" s="17">
+      <c r="AH44" s="23">
         <f t="shared" ref="AH43:AH48" si="51">S44/AE44</f>
         <v>0.81504016824332826</v>
       </c>
@@ -8105,7 +8105,7 @@
         <f t="shared" si="48"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AH45" s="17">
+      <c r="AH45" s="23">
         <f t="shared" si="51"/>
         <v>0.6819176734467306</v>
       </c>
@@ -8199,7 +8199,7 @@
         <f t="shared" si="48"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AH46" s="17">
+      <c r="AH46" s="23">
         <f t="shared" si="51"/>
         <v>0.59112951753920218</v>
       </c>
@@ -8293,7 +8293,7 @@
         <f t="shared" si="48"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AH47" s="17">
+      <c r="AH47" s="23">
         <f t="shared" si="51"/>
         <v>0.52319326181181025</v>
       </c>
@@ -8387,7 +8387,7 @@
         <f t="shared" si="48"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AH48" s="19">
+      <c r="AH48" s="47">
         <f t="shared" si="51"/>
         <v>0.47193411473704922</v>
       </c>
@@ -8681,14 +8681,14 @@
         <v>61.568000000000005</v>
       </c>
       <c r="T53" s="42">
-        <v>54.63</v>
+        <v>0.19020000000000001</v>
       </c>
       <c r="U53" s="17">
         <v>9.2420000000000002E-3</v>
       </c>
       <c r="V53" s="17">
         <f t="shared" si="53"/>
-        <v>54.639242000000003</v>
+        <v>0.19944200000000001</v>
       </c>
       <c r="W53" s="42">
         <v>9.2420000000000002E-3</v>
@@ -8712,7 +8712,7 @@
       </c>
       <c r="AC53" s="21">
         <f>Q53+T53+W53+Z53</f>
-        <v>109.26924200000001</v>
+        <v>54.829442</v>
       </c>
       <c r="AD53" s="21">
         <f>R53+U53+X53+AA53</f>
@@ -8720,19 +8720,19 @@
       </c>
       <c r="AE53" s="17">
         <f>AC53+AD53</f>
-        <v>116.21648400000001</v>
+        <v>61.776684000000003</v>
       </c>
       <c r="AF53" s="43">
         <f>Q53/AC53</f>
-        <v>0.49995770996562783</v>
+        <v>0.99636250173766139</v>
       </c>
       <c r="AG53" s="23">
         <f>R53/AD53</f>
         <v>0.99866968791356336</v>
       </c>
-      <c r="AH53" s="17">
+      <c r="AH53" s="23">
         <f>S53/AE53</f>
-        <v>0.5297699421021892</v>
+        <v>0.99662196177444551</v>
       </c>
       <c r="AJ53" s="1" t="s">
         <v>58</v>
@@ -8799,14 +8799,14 @@
         <v>1437.5</v>
       </c>
       <c r="T54" s="42">
-        <v>1271</v>
+        <v>28.88</v>
       </c>
       <c r="U54" s="17">
         <v>1.571</v>
       </c>
       <c r="V54" s="17">
         <f>T54+U54</f>
-        <v>1272.5709999999999</v>
+        <v>30.451000000000001</v>
       </c>
       <c r="W54" s="42">
         <v>1.571</v>
@@ -8830,7 +8830,7 @@
       </c>
       <c r="AC54" s="21">
         <f t="shared" ref="AC54:AD61" si="59">Q54+T54+W54+Z54</f>
-        <v>2543.5709999999999</v>
+        <v>1301.451</v>
       </c>
       <c r="AD54" s="21">
         <f t="shared" si="59"/>
@@ -8838,19 +8838,19 @@
       </c>
       <c r="AE54" s="17">
         <f t="shared" ref="AE54:AE61" si="60">AC54+AD54</f>
-        <v>2711.6695199999999</v>
+        <v>1469.54952</v>
       </c>
       <c r="AF54" s="43">
         <f t="shared" ref="AF54:AF61" si="61">Q54/AC54</f>
-        <v>0.49969118220014302</v>
+        <v>0.97660226931325111</v>
       </c>
       <c r="AG54" s="23">
         <f t="shared" ref="AG54:AG55" si="62">R54/AD54</f>
         <v>0.990490576597581</v>
       </c>
-      <c r="AH54" s="17">
+      <c r="AH54" s="23">
         <f t="shared" ref="AH54:AH56" si="63">S54/AE54</f>
-        <v>0.53011622153720273</v>
+        <v>0.97819092207250014</v>
       </c>
       <c r="AJ54" s="1"/>
     </row>
@@ -8913,14 +8913,14 @@
         <v>5314.9</v>
       </c>
       <c r="T55" s="42">
-        <v>4645</v>
+        <v>383.1</v>
       </c>
       <c r="U55" s="17">
         <v>24.64</v>
       </c>
       <c r="V55" s="17">
         <f>T55+U55</f>
-        <v>4669.6400000000003</v>
+        <v>407.74</v>
       </c>
       <c r="W55" s="42">
         <v>24.64</v>
@@ -8944,7 +8944,7 @@
       </c>
       <c r="AC55" s="21">
         <f t="shared" si="59"/>
-        <v>9314.6632799999988</v>
+        <v>5052.763280000001</v>
       </c>
       <c r="AD55" s="21">
         <f t="shared" si="59"/>
@@ -8952,19 +8952,19 @@
       </c>
       <c r="AE55" s="17">
         <f t="shared" si="60"/>
-        <v>10010.994559999999</v>
+        <v>5749.0945600000014</v>
       </c>
       <c r="AF55" s="43">
         <f t="shared" si="61"/>
-        <v>0.49867610458592987</v>
+        <v>0.91929895437333831</v>
       </c>
       <c r="AG55" s="23">
         <f t="shared" si="62"/>
         <v>0.96204209008103148</v>
       </c>
-      <c r="AH55" s="17">
+      <c r="AH55" s="23">
         <f t="shared" si="63"/>
-        <v>0.53090629189194161</v>
+        <v>0.92447601001017421</v>
       </c>
       <c r="AJ55" s="1"/>
     </row>
@@ -9027,14 +9027,14 @@
         <v>8212</v>
       </c>
       <c r="T56" s="42">
-        <v>7096</v>
+        <v>928.9</v>
       </c>
       <c r="U56" s="17">
         <v>69.36</v>
       </c>
       <c r="V56" s="17">
         <f>T56+U56</f>
-        <v>7165.36</v>
+        <v>998.26</v>
       </c>
       <c r="W56" s="42">
         <v>69.36</v>
@@ -9058,7 +9058,7 @@
       </c>
       <c r="AC56" s="21">
         <f t="shared" si="59"/>
-        <v>14261.5656</v>
+        <v>8094.4655999999995</v>
       </c>
       <c r="AD56" s="21">
         <f t="shared" si="59"/>
@@ -9066,19 +9066,19 @@
       </c>
       <c r="AE56" s="17">
         <f t="shared" si="60"/>
-        <v>15455.8032</v>
+        <v>9288.7031999999999</v>
       </c>
       <c r="AF56" s="43">
         <f t="shared" si="61"/>
-        <v>0.49756108123220355</v>
+        <v>0.87664836082569808</v>
       </c>
       <c r="AG56" s="23">
         <f t="shared" ref="AG56:AG61" si="65">R56/AD56</f>
         <v>0.93448740853578893</v>
       </c>
-      <c r="AH56" s="17">
+      <c r="AH56" s="23">
         <f t="shared" si="63"/>
-        <v>0.53132146506627365</v>
+        <v>0.88408465887897036</v>
       </c>
       <c r="AJ56" s="25">
         <f>4.77*306.39103*7</f>
@@ -9147,14 +9147,14 @@
         <v>10410</v>
       </c>
       <c r="T57" s="42">
-        <v>8896</v>
+        <v>1552</v>
       </c>
       <c r="U57" s="17">
         <v>130.4</v>
       </c>
       <c r="V57" s="17">
         <f t="shared" ref="V57:V61" si="67">T57+U57</f>
-        <v>9026.4</v>
+        <v>1682.4</v>
       </c>
       <c r="W57" s="42">
         <v>130.4</v>
@@ -9178,7 +9178,7 @@
       </c>
       <c r="AC57" s="21">
         <f t="shared" si="59"/>
-        <v>17923.196400000001</v>
+        <v>10579.196399999999</v>
       </c>
       <c r="AD57" s="21">
         <f t="shared" si="59"/>
@@ -9186,19 +9186,19 @@
       </c>
       <c r="AE57" s="17">
         <f t="shared" si="60"/>
-        <v>19591.0628</v>
+        <v>12247.0628</v>
       </c>
       <c r="AF57" s="43">
         <f t="shared" si="61"/>
-        <v>0.49634003898992035</v>
+        <v>0.84089562795147665</v>
       </c>
       <c r="AG57" s="23">
         <f t="shared" si="65"/>
         <v>0.90774656771069906</v>
       </c>
-      <c r="AH57" s="17">
+      <c r="AH57" s="23">
         <f t="shared" ref="AH56:AH61" si="68">S57/AE57</f>
-        <v>0.53136474045706183</v>
+        <v>0.84999972401545942</v>
       </c>
     </row>
     <row r="58" spans="1:54" x14ac:dyDescent="0.2">
@@ -9260,14 +9260,14 @@
         <v>14388</v>
       </c>
       <c r="T58" s="42">
-        <v>11890</v>
+        <v>3454</v>
       </c>
       <c r="U58" s="17">
         <v>395.2</v>
       </c>
       <c r="V58" s="17">
         <f t="shared" si="67"/>
-        <v>12285.2</v>
+        <v>3849.2</v>
       </c>
       <c r="W58" s="42">
         <v>395.2</v>
@@ -9291,7 +9291,7 @@
       </c>
       <c r="AC58" s="21">
         <f t="shared" si="59"/>
-        <v>24184.863000000001</v>
+        <v>15748.863000000001</v>
       </c>
       <c r="AD58" s="21">
         <f t="shared" si="59"/>
@@ -9299,19 +9299,19 @@
       </c>
       <c r="AE58" s="17">
         <f t="shared" si="60"/>
-        <v>27214.326000000001</v>
+        <v>18778.326000000001</v>
       </c>
       <c r="AF58" s="43">
         <f t="shared" si="61"/>
-        <v>0.49162982647451836</v>
+        <v>0.75497513693528218</v>
       </c>
       <c r="AG58" s="23">
         <f t="shared" si="65"/>
         <v>0.82456857865568922</v>
       </c>
-      <c r="AH58" s="17">
+      <c r="AH58" s="23">
         <f t="shared" si="68"/>
-        <v>0.52869213075495602</v>
+        <v>0.76620248258550838</v>
       </c>
     </row>
     <row r="59" spans="1:54" x14ac:dyDescent="0.2">
@@ -9363,24 +9363,24 @@
         <v>3334100</v>
       </c>
       <c r="Q59" s="42">
-        <v>2453000</v>
+        <v>12830</v>
       </c>
       <c r="R59" s="17">
         <v>3165</v>
       </c>
       <c r="S59" s="17">
         <f t="shared" si="52"/>
-        <v>2456165</v>
+        <v>15995</v>
       </c>
       <c r="T59" s="42">
-        <v>12830</v>
+        <v>5162</v>
       </c>
       <c r="U59" s="17">
         <v>722.2</v>
       </c>
       <c r="V59" s="17">
         <f t="shared" si="67"/>
-        <v>13552.2</v>
+        <v>5884.2</v>
       </c>
       <c r="W59" s="42">
         <v>5162</v>
@@ -9404,7 +9404,7 @@
       </c>
       <c r="AC59" s="21">
         <f t="shared" si="59"/>
-        <v>2472334</v>
+        <v>24496</v>
       </c>
       <c r="AD59" s="21">
         <f t="shared" si="59"/>
@@ -9412,19 +9412,19 @@
       </c>
       <c r="AE59" s="17">
         <f t="shared" si="60"/>
-        <v>2476554.35</v>
+        <v>28716.35</v>
       </c>
       <c r="AF59" s="43">
         <f t="shared" si="61"/>
-        <v>0.99217985919378204</v>
+        <v>0.5237589810581319</v>
       </c>
       <c r="AG59" s="23">
         <f t="shared" si="65"/>
         <v>0.74993780136718513</v>
       </c>
-      <c r="AH59" s="17">
+      <c r="AH59" s="23">
         <f t="shared" si="68"/>
-        <v>0.99176704924727366</v>
+        <v>0.55699975797759815</v>
       </c>
     </row>
     <row r="60" spans="1:54" x14ac:dyDescent="0.2">
@@ -9476,24 +9476,24 @@
         <v>3305000</v>
       </c>
       <c r="Q60" s="42">
-        <v>2427000</v>
+        <v>12860</v>
       </c>
       <c r="R60" s="17">
         <v>3580</v>
       </c>
       <c r="S60" s="17">
         <f t="shared" si="52"/>
-        <v>2430580</v>
+        <v>16440</v>
       </c>
       <c r="T60" s="42">
-        <v>12860</v>
+        <v>6515</v>
       </c>
       <c r="U60" s="17">
         <v>1083</v>
       </c>
       <c r="V60" s="17">
         <f t="shared" si="67"/>
-        <v>13943</v>
+        <v>7598</v>
       </c>
       <c r="W60" s="42">
         <v>6515</v>
@@ -9517,7 +9517,7 @@
       </c>
       <c r="AC60" s="21">
         <f t="shared" si="59"/>
-        <v>2448840</v>
+        <v>28355</v>
       </c>
       <c r="AD60" s="21">
         <f t="shared" si="59"/>
@@ -9525,19 +9525,19 @@
       </c>
       <c r="AE60" s="17">
         <f t="shared" si="60"/>
-        <v>2454092.75</v>
+        <v>33607.75</v>
       </c>
       <c r="AF60" s="43">
         <f t="shared" si="61"/>
-        <v>0.99108149164502379</v>
+        <v>0.4535355316522659</v>
       </c>
       <c r="AG60" s="23">
         <f t="shared" si="65"/>
         <v>0.68154776069677792</v>
       </c>
-      <c r="AH60" s="17">
+      <c r="AH60" s="23">
         <f t="shared" si="68"/>
-        <v>0.99041896440140664</v>
+        <v>0.48917288423057181</v>
       </c>
     </row>
     <row r="61" spans="1:54" s="18" customFormat="1" x14ac:dyDescent="0.2">
@@ -9589,24 +9589,24 @@
         <v>3273600</v>
       </c>
       <c r="Q61" s="42">
-        <v>2399000</v>
+        <v>12560</v>
       </c>
       <c r="R61" s="19">
         <v>3811</v>
       </c>
       <c r="S61" s="19">
         <f t="shared" si="52"/>
-        <v>2402811</v>
+        <v>16371</v>
       </c>
       <c r="T61" s="42">
-        <v>12560</v>
+        <v>7461</v>
       </c>
       <c r="U61" s="19">
         <v>1446</v>
       </c>
       <c r="V61" s="19">
         <f t="shared" si="67"/>
-        <v>14006</v>
+        <v>8907</v>
       </c>
       <c r="W61" s="42">
         <v>7461</v>
@@ -9630,7 +9630,7 @@
       </c>
       <c r="AC61" s="21">
         <f t="shared" si="59"/>
-        <v>2422708</v>
+        <v>31169</v>
       </c>
       <c r="AD61" s="21">
         <f t="shared" si="59"/>
@@ -9638,19 +9638,19 @@
       </c>
       <c r="AE61" s="19">
         <f t="shared" si="60"/>
-        <v>2428848</v>
+        <v>37309</v>
       </c>
       <c r="AF61" s="43">
         <f t="shared" si="61"/>
-        <v>0.99021425611340697</v>
+        <v>0.40296448394237866</v>
       </c>
       <c r="AG61" s="47">
         <f t="shared" si="65"/>
         <v>0.62068403908794789</v>
       </c>
-      <c r="AH61" s="19">
+      <c r="AH61" s="47">
         <f t="shared" si="68"/>
-        <v>0.98928010316001658</v>
+        <v>0.43879492883754589</v>
       </c>
     </row>
   </sheetData>

</xml_diff>